<commit_message>
automating Jason's excel script
</commit_message>
<xml_diff>
--- a/inputs/jason_template.xlsx
+++ b/inputs/jason_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11460" yWindow="460" windowWidth="12540" windowHeight="9880" tabRatio="884"/>
+    <workbookView xWindow="960" yWindow="460" windowWidth="23040" windowHeight="16120" tabRatio="884"/>
   </bookViews>
   <sheets>
     <sheet name="SFR ANALYSIS" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="146">
   <si>
     <t>Holding Costs</t>
   </si>
@@ -236,9 +236,6 @@
     <t>DATE:</t>
   </si>
   <si>
-    <t>123 Main St, Anywhere 95111</t>
-  </si>
-  <si>
     <t>MILES FROM SUBJECT</t>
   </si>
   <si>
@@ -387,9 +384,6 @@
   </si>
   <si>
     <t>PROPERTY DETAILS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ARV  </t>
   </si>
   <si>
     <t>Financing Costs (See Schedule)</t>
@@ -491,9 +485,6 @@
     <t>TYPE</t>
   </si>
   <si>
-    <t>MLS</t>
-  </si>
-  <si>
     <t>Price Range (2 yrs)</t>
   </si>
   <si>
@@ -535,9 +526,9 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="167" formatCode="0.0%"/>
-    <numFmt numFmtId="178" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="182" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
   <fonts count="59" x14ac:knownFonts="1">
     <font>
@@ -2274,13 +2265,13 @@
     <xf numFmtId="1" fontId="21" fillId="7" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="5" borderId="7" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="4" fillId="5" borderId="15" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="19" fillId="7" borderId="16" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="5" borderId="7" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="5" borderId="15" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="19" fillId="7" borderId="16" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="7" borderId="22" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2295,121 +2286,121 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="21" fillId="7" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="19" fillId="7" borderId="31" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="34" fillId="7" borderId="25" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="4" fillId="5" borderId="7" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="4" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="19" fillId="7" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="34" fillId="7" borderId="16" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="21" fillId="7" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="19" fillId="7" borderId="31" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="34" fillId="7" borderId="25" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="5" borderId="7" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="19" fillId="7" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="34" fillId="7" borderId="16" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="7" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="20" fillId="7" borderId="7" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="4" fillId="5" borderId="31" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="21" fillId="7" borderId="31" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="20" fillId="7" borderId="7" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="5" borderId="31" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="21" fillId="7" borderId="31" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="19" fillId="7" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="19" fillId="7" borderId="64" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="4" fillId="5" borderId="65" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="30" fillId="10" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="19" fillId="7" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="19" fillId="7" borderId="64" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="5" borderId="65" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="30" fillId="10" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="19" fillId="7" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="4" fillId="5" borderId="7" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="5" borderId="7" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="19" fillId="7" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="19" fillId="7" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="25" fillId="7" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="4" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="27" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="26" fillId="7" borderId="7" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="29" fillId="0" borderId="39" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="30" fillId="11" borderId="30" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="30" fillId="11" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="30" fillId="7" borderId="41" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="30" fillId="11" borderId="41" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="30" fillId="11" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="30" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="32" fillId="13" borderId="30" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="32" fillId="13" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="32" fillId="7" borderId="30" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="32" fillId="7" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="25" fillId="7" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="27" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="26" fillId="7" borderId="7" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="29" fillId="0" borderId="39" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="30" fillId="11" borderId="30" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="30" fillId="11" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="30" fillId="7" borderId="41" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="30" fillId="11" borderId="41" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="30" fillId="11" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="30" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="32" fillId="13" borderId="30" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="32" fillId="13" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="32" fillId="7" borderId="30" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="32" fillId="7" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="7" borderId="42" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="19" fillId="7" borderId="39" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="19" fillId="7" borderId="39" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="35" fillId="7" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="35" fillId="7" borderId="30" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="35" fillId="7" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="35" fillId="7" borderId="30" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="35" fillId="7" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="35" fillId="7" borderId="37" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2418,7 +2409,7 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="32" fillId="13" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="32" fillId="13" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2457,16 +2448,16 @@
     <xf numFmtId="0" fontId="36" fillId="7" borderId="21" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="29" fillId="12" borderId="30" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="29" fillId="12" borderId="41" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="29" fillId="7" borderId="30" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="29" fillId="7" borderId="41" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="29" fillId="12" borderId="30" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="29" fillId="12" borderId="41" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="29" fillId="7" borderId="30" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="29" fillId="7" borderId="41" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2565,10 +2556,10 @@
     <xf numFmtId="0" fontId="40" fillId="11" borderId="46" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="40" fillId="11" borderId="47" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="40" fillId="11" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="40" fillId="11" borderId="47" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="40" fillId="11" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2586,10 +2577,10 @@
     <xf numFmtId="0" fontId="5" fillId="9" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="41" fillId="14" borderId="21" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="41" fillId="14" borderId="21" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="41" fillId="14" borderId="24" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="41" fillId="14" borderId="24" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="29" fillId="12" borderId="30" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2667,13 +2658,13 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="15" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="43" fillId="7" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="44" fillId="7" borderId="7" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="43" fillId="7" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="44" fillId="7" borderId="7" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="45" fillId="7" borderId="7" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="45" fillId="7" borderId="7" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2682,7 +2673,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="46" fillId="7" borderId="26" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="46" fillId="7" borderId="26" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2716,7 +2707,7 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2735,10 +2726,10 @@
     <xf numFmtId="0" fontId="20" fillId="7" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="20" fillId="7" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="19" fillId="7" borderId="20" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="20" fillId="7" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="19" fillId="7" borderId="20" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="7" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2786,19 +2777,19 @@
     <xf numFmtId="0" fontId="29" fillId="12" borderId="33" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="29" fillId="12" borderId="57" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="29" fillId="12" borderId="57" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="29" fillId="12" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="4" fillId="5" borderId="26" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="5" borderId="26" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="48" fillId="7" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="48" fillId="7" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="32" fillId="0" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2807,94 +2798,94 @@
     <xf numFmtId="1" fontId="23" fillId="7" borderId="16" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="25" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="25" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="7" borderId="9" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="25" fillId="7" borderId="7" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="25" fillId="0" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="20" fillId="0" borderId="58" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="25" fillId="7" borderId="7" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="25" fillId="0" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="20" fillId="0" borderId="58" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="45" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="46" fillId="7" borderId="9" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="46" fillId="7" borderId="7" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="49" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="50" fillId="0" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="46" fillId="7" borderId="7" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="49" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="50" fillId="0" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="22" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="22" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="22" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="22" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="51" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="49" fillId="0" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="47" fillId="0" borderId="21" xfId="10" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="49" fillId="0" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="47" fillId="0" borderId="21" xfId="10" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="7" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="26" fillId="7" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="26" fillId="7" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="7" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="22" fillId="7" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="22" fillId="0" borderId="58" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="45" fillId="0" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="27" fillId="0" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="4" fillId="0" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="52" fillId="0" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="32" fillId="0" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="32" fillId="0" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="22" fillId="7" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="22" fillId="0" borderId="58" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="27" fillId="0" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="52" fillId="0" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="32" fillId="0" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="32" fillId="0" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2912,13 +2903,13 @@
     <xf numFmtId="0" fontId="20" fillId="8" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="20" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="45" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="52" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="20" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="52" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2933,31 +2924,16 @@
     <xf numFmtId="0" fontId="19" fillId="7" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="19" fillId="7" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="19" fillId="7" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="20" fillId="8" borderId="7" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="20" fillId="8" borderId="50" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="20" fillId="8" borderId="50" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="29" fillId="7" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2979,10 +2955,10 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="4" fillId="5" borderId="47" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="4" fillId="5" borderId="60" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="5" borderId="47" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="5" borderId="60" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="42" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2994,6 +2970,57 @@
     <xf numFmtId="0" fontId="42" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="14" borderId="9" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="14" borderId="20" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="56" fillId="8" borderId="9" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="56" fillId="8" borderId="31" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="56" fillId="8" borderId="20" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="12" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="12" borderId="0" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="7" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="7" borderId="0" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3012,18 +3039,6 @@
     <xf numFmtId="0" fontId="58" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="57" fillId="7" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="7" borderId="0" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="12" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="12" borderId="0" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="57" fillId="7" borderId="6" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3040,30 +3055,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="14" borderId="9" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="14" borderId="20" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="56" fillId="8" borderId="9" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="56" fillId="8" borderId="31" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="56" fillId="8" borderId="20" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3080,7 +3071,67 @@
     <cellStyle name="Normal 2" xfId="9"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFC00000"/>
@@ -4128,7 +4179,7 @@
   <dimension ref="A1:L217"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="E122" sqref="E122"/>
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
@@ -4153,11 +4204,11 @@
       <c r="I1" s="30"/>
     </row>
     <row r="2" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="373" t="s">
-        <v>135</v>
-      </c>
-      <c r="B2" s="373"/>
-      <c r="C2" s="373"/>
+      <c r="A2" s="368" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" s="368"/>
+      <c r="C2" s="368"/>
       <c r="E2"/>
       <c r="F2"/>
       <c r="G2"/>
@@ -4167,9 +4218,9 @@
       <c r="K2"/>
     </row>
     <row r="3" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="373"/>
-      <c r="B3" s="373"/>
-      <c r="C3" s="373"/>
+      <c r="A3" s="368"/>
+      <c r="B3" s="368"/>
+      <c r="C3" s="368"/>
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3"/>
@@ -4189,7 +4240,7 @@
     </row>
     <row r="5" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="82" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B5" s="82"/>
       <c r="C5" s="42"/>
@@ -4202,8 +4253,8 @@
       <c r="K5"/>
     </row>
     <row r="6" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E6" s="378"/>
-      <c r="F6" s="378"/>
+      <c r="E6" s="373"/>
+      <c r="F6" s="373"/>
       <c r="G6"/>
       <c r="H6"/>
       <c r="I6"/>
@@ -4211,11 +4262,11 @@
       <c r="K6"/>
     </row>
     <row r="7" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="379" t="s">
+      <c r="A7" s="374" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="378"/>
-      <c r="F7" s="378"/>
+      <c r="E7" s="373"/>
+      <c r="F7" s="373"/>
       <c r="G7"/>
       <c r="H7"/>
       <c r="I7"/>
@@ -4223,7 +4274,7 @@
       <c r="K7"/>
     </row>
     <row r="8" spans="1:11" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="379"/>
+      <c r="A8" s="374"/>
       <c r="D8" s="42"/>
       <c r="E8"/>
       <c r="F8"/>
@@ -4235,7 +4286,7 @@
     </row>
     <row r="9" spans="1:11" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A9" s="260" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B9" s="27"/>
       <c r="C9" s="28"/>
@@ -4249,10 +4300,10 @@
     </row>
     <row r="10" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="264" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B10" s="272" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C10" s="273"/>
       <c r="E10"/>
@@ -4265,7 +4316,7 @@
     </row>
     <row r="11" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="265" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B11" s="153">
         <v>350000</v>
@@ -4285,10 +4336,10 @@
     </row>
     <row r="12" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="265" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B12" s="267" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C12" s="304"/>
       <c r="E12"/>
@@ -4301,10 +4352,10 @@
     </row>
     <row r="13" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="305" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B13" s="115" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C13" s="306"/>
       <c r="E13"/>
@@ -4317,7 +4368,7 @@
     </row>
     <row r="14" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="305" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B14" s="74">
         <v>3</v>
@@ -4333,7 +4384,7 @@
     </row>
     <row r="15" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="305" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B15" s="74">
         <v>2</v>
@@ -4351,10 +4402,10 @@
       <c r="A16" s="266" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="380">
+      <c r="B16" s="375">
         <v>42375</v>
       </c>
-      <c r="C16" s="381"/>
+      <c r="C16" s="376"/>
       <c r="E16"/>
       <c r="F16"/>
       <c r="G16"/>
@@ -4373,7 +4424,7 @@
       <c r="K17"/>
     </row>
     <row r="18" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="371" t="s">
+      <c r="A18" s="383" t="s">
         <v>35</v>
       </c>
       <c r="E18"/>
@@ -4385,7 +4436,7 @@
       <c r="K18"/>
     </row>
     <row r="19" spans="1:11" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="372"/>
+      <c r="A19" s="384"/>
       <c r="E19"/>
       <c r="F19"/>
       <c r="G19"/>
@@ -4396,7 +4447,7 @@
     </row>
     <row r="20" spans="1:11" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A20" s="301" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B20" s="28"/>
       <c r="E20"/>
@@ -4422,7 +4473,7 @@
     </row>
     <row r="22" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="44" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B22" s="34">
         <v>1956</v>
@@ -4437,7 +4488,7 @@
     </row>
     <row r="23" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B23" s="35">
         <v>6305</v>
@@ -4452,7 +4503,7 @@
     </row>
     <row r="24" spans="1:11" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A24" s="45" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B24" s="36">
         <v>1970</v>
@@ -4526,8 +4577,8 @@
         <f>(B22*B27)+B22</f>
         <v>2249.4</v>
       </c>
-      <c r="E29" s="378"/>
-      <c r="F29" s="378"/>
+      <c r="E29" s="373"/>
+      <c r="F29" s="373"/>
       <c r="G29"/>
       <c r="H29"/>
       <c r="I29"/>
@@ -4635,19 +4686,19 @@
       <c r="L36" s="43"/>
     </row>
     <row r="37" spans="1:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="368" t="s">
-        <v>145</v>
-      </c>
-      <c r="B37" s="369"/>
-      <c r="C37" s="369"/>
-      <c r="D37" s="369"/>
-      <c r="E37" s="369"/>
-      <c r="F37" s="369"/>
-      <c r="G37" s="369"/>
-      <c r="H37" s="369"/>
-      <c r="I37" s="369"/>
-      <c r="J37" s="369"/>
-      <c r="K37" s="370"/>
+      <c r="A37" s="380" t="s">
+        <v>142</v>
+      </c>
+      <c r="B37" s="381"/>
+      <c r="C37" s="381"/>
+      <c r="D37" s="381"/>
+      <c r="E37" s="381"/>
+      <c r="F37" s="381"/>
+      <c r="G37" s="381"/>
+      <c r="H37" s="381"/>
+      <c r="I37" s="381"/>
+      <c r="J37" s="381"/>
+      <c r="K37" s="382"/>
       <c r="L37" s="43"/>
     </row>
     <row r="38" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -4676,55 +4727,39 @@
         <v>28</v>
       </c>
       <c r="I38" s="93" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J38" s="94" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K38" s="353" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="L38" s="43"/>
     </row>
     <row r="39" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="116" t="s">
-        <v>66</v>
-      </c>
-      <c r="B39" s="160">
-        <v>265000</v>
-      </c>
-      <c r="C39" s="141">
-        <v>1991</v>
-      </c>
-      <c r="D39" s="288">
+        <v>67</v>
+      </c>
+      <c r="B39" s="160"/>
+      <c r="C39" s="141"/>
+      <c r="D39" s="288" t="e">
         <f>B39/C39</f>
-        <v>133.09894525364138</v>
-      </c>
-      <c r="E39" s="79">
-        <v>5900</v>
-      </c>
-      <c r="F39" s="74">
-        <v>2000</v>
-      </c>
-      <c r="G39" s="73">
-        <v>30</v>
-      </c>
-      <c r="H39" s="90">
-        <v>36526</v>
-      </c>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E39" s="79"/>
+      <c r="F39" s="74"/>
+      <c r="G39" s="73"/>
+      <c r="H39" s="90"/>
       <c r="I39" s="309">
-        <v>0.5</v>
-      </c>
-      <c r="J39" s="73" t="s">
-        <v>117</v>
-      </c>
-      <c r="K39" s="354" t="s">
-        <v>137</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J39" s="73"/>
+      <c r="K39" s="73"/>
     </row>
     <row r="40" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="116" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B40" s="160"/>
       <c r="C40" s="141"/>
@@ -4737,7 +4772,7 @@
       <c r="G40" s="73"/>
       <c r="H40" s="90"/>
       <c r="I40" s="309">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="J40" s="73"/>
       <c r="K40" s="354"/>
@@ -4745,7 +4780,7 @@
     </row>
     <row r="41" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="116" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B41" s="160"/>
       <c r="C41" s="141"/>
@@ -4758,7 +4793,7 @@
       <c r="G41" s="73"/>
       <c r="H41" s="90"/>
       <c r="I41" s="309">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="J41" s="73"/>
       <c r="K41" s="354"/>
@@ -4766,7 +4801,7 @@
     </row>
     <row r="42" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="116" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B42" s="160"/>
       <c r="C42" s="141"/>
@@ -4787,7 +4822,7 @@
     </row>
     <row r="43" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="116" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B43" s="160"/>
       <c r="C43" s="141"/>
@@ -4808,7 +4843,7 @@
     </row>
     <row r="44" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="116" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B44" s="160"/>
       <c r="C44" s="141"/>
@@ -4829,7 +4864,7 @@
     </row>
     <row r="45" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="116" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B45" s="160"/>
       <c r="C45" s="141"/>
@@ -4850,7 +4885,7 @@
     </row>
     <row r="46" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="116" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B46" s="160"/>
       <c r="C46" s="141"/>
@@ -4871,7 +4906,7 @@
     </row>
     <row r="47" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="116" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B47" s="160"/>
       <c r="C47" s="141"/>
@@ -4892,7 +4927,7 @@
     </row>
     <row r="48" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="116" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B48" s="160"/>
       <c r="C48" s="141"/>
@@ -4913,7 +4948,7 @@
     </row>
     <row r="49" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="116" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B49" s="160"/>
       <c r="C49" s="141"/>
@@ -4941,7 +4976,7 @@
         <v>22</v>
       </c>
       <c r="D50" s="65" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E50" s="75" t="s">
         <v>55</v>
@@ -4960,29 +4995,29 @@
     </row>
     <row r="51" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="117"/>
-      <c r="B51" s="161">
+      <c r="B51" s="161" t="e">
         <f>AVERAGE(B39:B49)</f>
-        <v>265000</v>
-      </c>
-      <c r="C51" s="142">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C51" s="142" t="e">
         <f>AVERAGE(C39:C49)</f>
-        <v>1991</v>
-      </c>
-      <c r="D51" s="289">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D51" s="289" t="e">
         <f>B51/C51</f>
-        <v>133.09894525364138</v>
-      </c>
-      <c r="E51" s="89">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E51" s="89" t="e">
         <f>AVERAGE(E39:E49)</f>
-        <v>5900</v>
-      </c>
-      <c r="F51" s="75">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F51" s="75" t="e">
         <f>AVERAGE(F39:F49)</f>
-        <v>2000</v>
-      </c>
-      <c r="G51" s="75">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G51" s="75" t="e">
         <f>AVERAGE(G39:G49)</f>
-        <v>30</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="H51" s="30"/>
       <c r="I51" s="30"/>
@@ -5005,16 +5040,16 @@
     </row>
     <row r="53" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="261" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B53" s="262"/>
       <c r="C53" s="66"/>
-      <c r="D53" s="382" t="s">
-        <v>146</v>
-      </c>
-      <c r="E53" s="383"/>
-      <c r="F53" s="383"/>
-      <c r="G53" s="384"/>
+      <c r="D53" s="377" t="s">
+        <v>143</v>
+      </c>
+      <c r="E53" s="378"/>
+      <c r="F53" s="378"/>
+      <c r="G53" s="379"/>
       <c r="H53" s="30"/>
       <c r="I53" s="30"/>
       <c r="J53" s="30"/>
@@ -5024,19 +5059,19 @@
       <c r="A54" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B54" s="159">
+      <c r="B54" s="159" t="e">
         <f>B57*B22</f>
-        <v>260341.53691612254</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="C54" s="30"/>
       <c r="D54" s="20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E54" s="74">
         <v>5500</v>
       </c>
       <c r="F54" s="20" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="G54" s="74">
         <v>3</v>
@@ -5048,21 +5083,21 @@
     </row>
     <row r="55" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="B55" s="162">
+        <v>105</v>
+      </c>
+      <c r="B55" s="162" t="e">
         <f>C51</f>
-        <v>1991</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="C55" s="30"/>
       <c r="D55" s="20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E55" s="74">
         <v>1150</v>
       </c>
       <c r="F55" s="20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G55" s="74">
         <v>2</v>
@@ -5074,21 +5109,21 @@
     </row>
     <row r="56" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="B56" s="299">
+        <v>106</v>
+      </c>
+      <c r="B56" s="299" t="e">
         <f>B51</f>
-        <v>265000</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="C56" s="66"/>
       <c r="D56" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="E56" s="74" t="s">
         <v>138</v>
       </c>
-      <c r="E56" s="74" t="s">
-        <v>141</v>
-      </c>
       <c r="F56" s="20" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="G56" s="74">
         <v>1937</v>
@@ -5100,21 +5135,21 @@
     </row>
     <row r="57" spans="1:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A57" s="184" t="s">
-        <v>84</v>
-      </c>
-      <c r="B57" s="185">
+        <v>83</v>
+      </c>
+      <c r="B57" s="185" t="e">
         <f>D51</f>
-        <v>133.09894525364138</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="C57" s="67"/>
       <c r="D57" s="300" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E57" s="317">
         <v>450000</v>
       </c>
       <c r="F57" s="300" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G57" s="118">
         <v>79</v>
@@ -5129,16 +5164,16 @@
       <c r="D58" s="54"/>
     </row>
     <row r="59" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A59" s="371" t="s">
+      <c r="A59" s="383" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="60" spans="1:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="372"/>
+      <c r="A60" s="384"/>
     </row>
     <row r="61" spans="1:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A61" s="301" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B61" s="28"/>
     </row>
@@ -5170,13 +5205,13 @@
     </row>
     <row r="65" spans="1:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A65" s="85" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B65" s="86"/>
     </row>
     <row r="66" spans="1:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A66" s="301" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B66" s="302"/>
     </row>
@@ -5226,18 +5261,18 @@
       <c r="I70" s="54"/>
     </row>
     <row r="71" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A71" s="371" t="s">
+      <c r="A71" s="383" t="s">
         <v>37</v>
       </c>
       <c r="E71"/>
       <c r="F71"/>
       <c r="G71"/>
-      <c r="H71" s="378"/>
-      <c r="I71" s="378"/>
+      <c r="H71" s="373"/>
+      <c r="I71" s="373"/>
       <c r="J71"/>
     </row>
     <row r="72" spans="1:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="372"/>
+      <c r="A72" s="384"/>
       <c r="E72"/>
       <c r="F72"/>
       <c r="G72"/>
@@ -5247,7 +5282,7 @@
     </row>
     <row r="73" spans="1:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A73" s="360" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B73" s="362"/>
       <c r="C73" s="362"/>
@@ -5263,15 +5298,15 @@
       <c r="A74" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B74" s="150">
+      <c r="B74" s="150" t="e">
         <f>B54</f>
-        <v>260341.53691612254</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="C74" s="146" t="s">
         <v>31</v>
       </c>
       <c r="D74" s="158" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E74"/>
       <c r="F74"/>
@@ -5292,9 +5327,9 @@
         <f>B75</f>
         <v>88020</v>
       </c>
-      <c r="D75" s="145">
+      <c r="D75" s="145" t="e">
         <f>B74-B75</f>
-        <v>172321.53691612254</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="E75"/>
       <c r="F75"/>
@@ -5305,18 +5340,18 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A76" s="10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B76" s="11">
         <v>0.06</v>
       </c>
-      <c r="C76" s="151">
+      <c r="C76" s="151" t="e">
         <f xml:space="preserve"> B76*B74</f>
-        <v>15620.492214967351</v>
-      </c>
-      <c r="D76" s="145">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D76" s="145" t="e">
         <f t="shared" ref="D76:D81" si="1">D75-C76</f>
-        <v>156701.04470115519</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="E76"/>
       <c r="F76"/>
@@ -5332,13 +5367,13 @@
       <c r="B77" s="11">
         <v>0.03</v>
       </c>
-      <c r="C77" s="151">
+      <c r="C77" s="151" t="e">
         <f>B77*B74</f>
-        <v>7810.2461074836756</v>
-      </c>
-      <c r="D77" s="145">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D77" s="145" t="e">
         <f t="shared" si="1"/>
-        <v>148890.79859367153</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="E77"/>
       <c r="F77"/>
@@ -5354,13 +5389,13 @@
       <c r="B78" s="143">
         <v>0.03</v>
       </c>
-      <c r="C78" s="151">
+      <c r="C78" s="151" t="e">
         <f>B78*B74</f>
-        <v>7810.2461074836756</v>
-      </c>
-      <c r="D78" s="145">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D78" s="145" t="e">
         <f t="shared" si="1"/>
-        <v>141080.55248618784</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="E78"/>
       <c r="F78"/>
@@ -5376,13 +5411,13 @@
       <c r="B79" s="11">
         <v>0.1</v>
       </c>
-      <c r="C79" s="151">
+      <c r="C79" s="151" t="e">
         <f>B79*B74</f>
-        <v>26034.153691612257</v>
-      </c>
-      <c r="D79" s="145">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D79" s="145" t="e">
         <f t="shared" si="1"/>
-        <v>115046.39879457558</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="E79"/>
       <c r="F79"/>
@@ -5393,7 +5428,7 @@
     </row>
     <row r="80" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A80" s="363" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B80" s="153">
         <v>0</v>
@@ -5402,9 +5437,9 @@
         <f>B80</f>
         <v>0</v>
       </c>
-      <c r="D80" s="364">
+      <c r="D80" s="364" t="e">
         <f t="shared" si="1"/>
-        <v>115046.39879457558</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="E80"/>
       <c r="F80"/>
@@ -5424,9 +5459,9 @@
         <f>B81</f>
         <v>15000</v>
       </c>
-      <c r="D81" s="157">
+      <c r="D81" s="157" t="e">
         <f t="shared" si="1"/>
-        <v>100046.39879457558</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="E81"/>
       <c r="F81"/>
@@ -5439,13 +5474,13 @@
       <c r="A82" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="B82" s="274">
+      <c r="B82" s="274" t="e">
         <f>B74-(C75+C76+C77+C78+C79+C81+C80)</f>
-        <v>100046.39879457559</v>
-      </c>
-      <c r="C82" s="152">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C82" s="152" t="e">
         <f>SUM(C75:C81)</f>
-        <v>160295.13812154694</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="D82" s="149"/>
       <c r="E82"/>
@@ -5459,12 +5494,12 @@
       <c r="A83" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="B83" s="154">
+      <c r="B83" s="154" t="e">
         <f>C79</f>
-        <v>26034.153691612257</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="C83" s="263" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D83" s="31"/>
       <c r="E83"/>
@@ -5476,11 +5511,11 @@
     </row>
     <row r="84" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A84" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="B84" s="155">
+        <v>118</v>
+      </c>
+      <c r="B84" s="155" t="e">
         <f>C75+C76+C77+C78+C81+C80</f>
-        <v>134260.9844299347</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="C84" s="147" t="s">
         <v>10</v>
@@ -5547,16 +5582,16 @@
       <c r="J88"/>
     </row>
     <row r="89" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A89" s="371" t="s">
+      <c r="A89" s="383" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="90" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="372"/>
+      <c r="A90" s="384"/>
     </row>
     <row r="91" spans="1:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A91" s="301" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B91" s="303"/>
       <c r="C91" s="303"/>
@@ -5578,16 +5613,16 @@
         <v>12</v>
       </c>
       <c r="E92" s="277" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F92" s="278" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A93" s="168">
+      <c r="A93" s="168" t="e">
         <f>B74</f>
-        <v>260341.53691612254</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="B93" s="166">
         <f>B64</f>
@@ -5599,13 +5634,13 @@
       <c r="D93" s="9">
         <v>0.75</v>
       </c>
-      <c r="E93" s="275">
+      <c r="E93" s="275" t="e">
         <f>(A93*D93)-B63-C93</f>
-        <v>92236.152687091904</v>
-      </c>
-      <c r="F93" s="280">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F93" s="280" t="e">
         <f>E93/B22</f>
-        <v>47.155497283789316</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="94" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -5613,17 +5648,17 @@
         <v>33</v>
       </c>
       <c r="B94" s="76"/>
-      <c r="C94" s="376" t="s">
-        <v>70</v>
-      </c>
-      <c r="D94" s="377"/>
-      <c r="E94" s="276">
+      <c r="C94" s="371" t="s">
+        <v>69</v>
+      </c>
+      <c r="D94" s="372"/>
+      <c r="E94" s="276" t="e">
         <f>(E93+E95)/2</f>
-        <v>87624.345052737306</v>
-      </c>
-      <c r="F94" s="281">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F94" s="281" t="e">
         <f>E94/B22</f>
-        <v>44.79772241959985</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="95" spans="1:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
@@ -5631,27 +5666,27 @@
         <v>39</v>
       </c>
       <c r="B95" s="77"/>
-      <c r="C95" s="374" t="s">
+      <c r="C95" s="369" t="s">
         <v>58</v>
       </c>
-      <c r="D95" s="375"/>
-      <c r="E95" s="279">
+      <c r="D95" s="370"/>
+      <c r="E95" s="279" t="e">
         <f>E93*0.9</f>
-        <v>83012.537418382723</v>
-      </c>
-      <c r="F95" s="282">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F95" s="282" t="e">
         <f>E95/B22</f>
-        <v>42.439947555410392</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A97" s="371" t="s">
+      <c r="A97" s="383" t="s">
         <v>40</v>
       </c>
       <c r="B97" s="13"/>
     </row>
     <row r="98" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="372"/>
+      <c r="A98" s="384"/>
       <c r="B98" s="81"/>
     </row>
     <row r="99" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -5660,7 +5695,7 @@
       </c>
       <c r="B99" s="287"/>
       <c r="C99" s="295" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D99"/>
       <c r="E99"/>
@@ -5669,13 +5704,13 @@
       <c r="A100" s="297" t="s">
         <v>11</v>
       </c>
-      <c r="B100" s="298">
+      <c r="B100" s="298" t="e">
         <f>B74</f>
-        <v>260341.53691612254</v>
-      </c>
-      <c r="C100" s="328">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C100" s="328" t="e">
         <f>B100/B22</f>
-        <v>133.09894525364138</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="D100" s="23"/>
       <c r="E100" s="23"/>
@@ -5685,13 +5720,13 @@
       <c r="A101" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="B101" s="169">
+      <c r="B101" s="169" t="e">
         <f>B84</f>
-        <v>134260.9844299347</v>
-      </c>
-      <c r="C101" s="327">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C101" s="327" t="e">
         <f>B101/B22</f>
-        <v>68.640585086878687</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="D101" s="23"/>
       <c r="E101" s="23"/>
@@ -5702,13 +5737,13 @@
       <c r="A102" s="323" t="s">
         <v>54</v>
       </c>
-      <c r="B102" s="324">
+      <c r="B102" s="324" t="e">
         <f>B82</f>
-        <v>100046.39879457559</v>
-      </c>
-      <c r="C102" s="327">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C102" s="327" t="e">
         <f>B102/B22</f>
-        <v>51.148465641398566</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="D102" s="23"/>
       <c r="E102" s="23"/>
@@ -5719,13 +5754,13 @@
       <c r="A103" s="325" t="s">
         <v>62</v>
       </c>
-      <c r="B103" s="326">
+      <c r="B103" s="326" t="e">
         <f>E93</f>
-        <v>92236.152687091904</v>
-      </c>
-      <c r="C103" s="327">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C103" s="327" t="e">
         <f>B103/B22</f>
-        <v>47.155497283789316</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="D103" s="23"/>
       <c r="E103" s="23"/>
@@ -5745,13 +5780,13 @@
       <c r="A105" s="329" t="s">
         <v>54</v>
       </c>
-      <c r="B105" s="330">
+      <c r="B105" s="330" t="e">
         <f>B82</f>
-        <v>100046.39879457559</v>
-      </c>
-      <c r="C105" s="346">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C105" s="346" t="e">
         <f>B105/B22</f>
-        <v>51.148465641398566</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="D105" s="290"/>
       <c r="E105" s="291"/>
@@ -5762,13 +5797,13 @@
       <c r="A106" s="80" t="s">
         <v>61</v>
       </c>
-      <c r="B106" s="171">
+      <c r="B106" s="171" t="e">
         <f>B105*0.9</f>
-        <v>90041.758915118044</v>
-      </c>
-      <c r="C106" s="347">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C106" s="347" t="e">
         <f>B106/B22</f>
-        <v>46.033619077258713</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="D106" s="23"/>
       <c r="E106" s="23"/>
@@ -5777,13 +5812,13 @@
       <c r="A107" s="80" t="s">
         <v>64</v>
       </c>
-      <c r="B107" s="171">
+      <c r="B107" s="171" t="e">
         <f>B100-(B106+B101)</f>
-        <v>36038.793571069778</v>
-      </c>
-      <c r="C107" s="347">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C107" s="347" t="e">
         <f>B107/B22</f>
-        <v>18.424741089503975</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="D107" s="23"/>
       <c r="E107" s="23"/>
@@ -5794,13 +5829,13 @@
       <c r="A108" s="138" t="s">
         <v>60</v>
       </c>
-      <c r="B108" s="171">
+      <c r="B108" s="171" t="e">
         <f>B100-(B105+B101)</f>
-        <v>26034.153691612242</v>
-      </c>
-      <c r="C108" s="347">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C108" s="347" t="e">
         <f>B108/B22</f>
-        <v>13.309894525364133</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="D108" s="23"/>
       <c r="E108" s="23"/>
@@ -5818,13 +5853,13 @@
       <c r="A110" s="331" t="s">
         <v>62</v>
       </c>
-      <c r="B110" s="332">
+      <c r="B110" s="332" t="e">
         <f>E93</f>
-        <v>92236.152687091904</v>
-      </c>
-      <c r="C110" s="349">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C110" s="349" t="e">
         <f>B110/B22</f>
-        <v>47.155497283789316</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="D110" s="23"/>
       <c r="E110" s="23"/>
@@ -5835,13 +5870,13 @@
       <c r="A111" s="69" t="s">
         <v>59</v>
       </c>
-      <c r="B111" s="172">
+      <c r="B111" s="172" t="e">
         <f>E95</f>
-        <v>83012.537418382723</v>
-      </c>
-      <c r="C111" s="350">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C111" s="350" t="e">
         <f>B111/B22</f>
-        <v>42.439947555410392</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="D111" s="23"/>
       <c r="E111" s="23"/>
@@ -5852,13 +5887,13 @@
       <c r="A112" s="139" t="s">
         <v>63</v>
       </c>
-      <c r="B112" s="172">
+      <c r="B112" s="172" t="e">
         <f>B100-B110-B101</f>
-        <v>33844.399799095932</v>
-      </c>
-      <c r="C112" s="350">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C112" s="350" t="e">
         <f>B112/B22</f>
-        <v>17.302862882973379</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="D112" s="23"/>
       <c r="E112" s="23"/>
@@ -5904,16 +5939,16 @@
       <c r="A116" s="343" t="s">
         <v>11</v>
       </c>
-      <c r="B116" s="344">
+      <c r="B116" s="344" t="e">
         <f>B100</f>
-        <v>260341.53691612254</v>
-      </c>
-      <c r="C116" s="345">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C116" s="345" t="e">
         <f>C100</f>
-        <v>133.09894525364138</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="D116" s="356" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E116" s="23"/>
       <c r="G116" s="30"/>
@@ -5921,19 +5956,19 @@
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A117" s="335" t="s">
-        <v>131</v>
-      </c>
-      <c r="B117" s="336">
+        <v>129</v>
+      </c>
+      <c r="B117" s="336" t="e">
         <f>B102+B101</f>
-        <v>234307.3832245103</v>
-      </c>
-      <c r="C117" s="337">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C117" s="337" t="e">
         <f>C102+C101</f>
-        <v>119.78905072827726</v>
-      </c>
-      <c r="D117" s="357">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D117" s="357" t="e">
         <f>B116-B117</f>
-        <v>26034.153691612242</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="E117" s="23"/>
       <c r="G117" s="30"/>
@@ -5941,19 +5976,19 @@
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A118" s="338" t="s">
-        <v>132</v>
-      </c>
-      <c r="B118" s="333">
+        <v>130</v>
+      </c>
+      <c r="B118" s="333" t="e">
         <f>B103+B101</f>
-        <v>226497.13711702661</v>
-      </c>
-      <c r="C118" s="339">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C118" s="339" t="e">
         <f>C103+C101</f>
-        <v>115.796082370668</v>
-      </c>
-      <c r="D118" s="358">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D118" s="358" t="e">
         <f>B116-B118</f>
-        <v>33844.399799095932</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="E118" s="23"/>
       <c r="G118" s="30"/>
@@ -5961,26 +5996,26 @@
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A119" s="296" t="s">
-        <v>133</v>
-      </c>
-      <c r="B119" s="340">
+        <v>131</v>
+      </c>
+      <c r="B119" s="340" t="e">
         <f>E95+B101</f>
-        <v>217273.52184831741</v>
-      </c>
-      <c r="C119" s="334">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C119" s="334" t="e">
         <f>F95+C101</f>
-        <v>111.08053264228909</v>
-      </c>
-      <c r="D119" s="359">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D119" s="359" t="e">
         <f>B116-B119</f>
-        <v>43068.015067805129</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="E119" s="23"/>
       <c r="H119" s="30"/>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A120" s="251" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B120" s="252"/>
       <c r="C120" s="253"/>
@@ -6282,6 +6317,7 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A97:A98"/>
     <mergeCell ref="A2:C3"/>
     <mergeCell ref="C95:D95"/>
     <mergeCell ref="C94:D94"/>
@@ -6296,29 +6332,28 @@
     <mergeCell ref="A59:A60"/>
     <mergeCell ref="A71:A72"/>
     <mergeCell ref="A89:A90"/>
-    <mergeCell ref="A97:A98"/>
   </mergeCells>
   <conditionalFormatting sqref="C39:C49">
-    <cfRule type="cellIs" dxfId="5" priority="11" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="11" stopIfTrue="1" operator="lessThan">
       <formula>$B$28</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="12" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="12" stopIfTrue="1" operator="greaterThan">
       <formula>$B$29</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E39:E49">
-    <cfRule type="cellIs" dxfId="3" priority="17" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="17" stopIfTrue="1" operator="lessThan">
       <formula>$B$31</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="18" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="18" stopIfTrue="1" operator="greaterThan">
       <formula>$B$32</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F39:F49">
-    <cfRule type="cellIs" dxfId="1" priority="23" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="23" stopIfTrue="1" operator="lessThan">
       <formula>$B$34</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="24" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="24" stopIfTrue="1" operator="greaterThan">
       <formula>$B$35</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6352,34 +6387,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="385" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" s="386"/>
-      <c r="C1" s="386"/>
-      <c r="D1" s="386"/>
-      <c r="E1" s="386"/>
-      <c r="F1" s="387"/>
+      <c r="A1" s="397" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="398"/>
+      <c r="C1" s="398"/>
+      <c r="D1" s="398"/>
+      <c r="E1" s="398"/>
+      <c r="F1" s="399"/>
     </row>
     <row r="2" spans="1:13" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="388"/>
-      <c r="B2" s="389"/>
-      <c r="C2" s="389"/>
-      <c r="D2" s="389"/>
-      <c r="E2" s="389"/>
-      <c r="F2" s="390"/>
+      <c r="A2" s="400"/>
+      <c r="B2" s="401"/>
+      <c r="C2" s="401"/>
+      <c r="D2" s="401"/>
+      <c r="E2" s="401"/>
+      <c r="F2" s="402"/>
     </row>
     <row r="3" spans="1:13" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="218" t="str">
         <f>'SFR ANALYSIS'!A10:B10</f>
         <v xml:space="preserve">ADDRESS:  </v>
       </c>
-      <c r="B3" s="399" t="str">
+      <c r="B3" s="407" t="str">
         <f>'SFR ANALYSIS'!B10:C10</f>
         <v>123 Main St, Anywhere CA 91234</v>
       </c>
-      <c r="C3" s="399"/>
-      <c r="D3" s="400"/>
+      <c r="C3" s="407"/>
+      <c r="D3" s="408"/>
       <c r="E3" s="202" t="s">
         <v>53</v>
       </c>
@@ -6389,20 +6424,20 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="406" t="s">
-        <v>134</v>
-      </c>
-      <c r="B4" s="407"/>
-      <c r="C4" s="407"/>
-      <c r="D4" s="407"/>
-      <c r="E4" s="407"/>
-      <c r="F4" s="408"/>
+      <c r="A4" s="390" t="s">
+        <v>132</v>
+      </c>
+      <c r="B4" s="391"/>
+      <c r="C4" s="391"/>
+      <c r="D4" s="391"/>
+      <c r="E4" s="391"/>
+      <c r="F4" s="392"/>
     </row>
     <row r="5" spans="1:13" ht="16" x14ac:dyDescent="0.15">
-      <c r="A5" s="397" t="s">
+      <c r="A5" s="405" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="398"/>
+      <c r="B5" s="406"/>
       <c r="C5" s="203" t="s">
         <v>20</v>
       </c>
@@ -6413,40 +6448,40 @@
         <v>21</v>
       </c>
       <c r="F5" s="219" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="16" x14ac:dyDescent="0.15">
       <c r="A6" s="393" t="str">
         <f>'SFR ANALYSIS'!A39</f>
-        <v>123 Main St, Anywhere 95111</v>
+        <v>N/A</v>
       </c>
       <c r="B6" s="394"/>
       <c r="C6" s="204">
         <f>'SFR ANALYSIS'!B39</f>
-        <v>265000</v>
+        <v>0</v>
       </c>
       <c r="D6" s="249">
         <f>'SFR ANALYSIS'!C39</f>
-        <v>1991</v>
-      </c>
-      <c r="E6" s="205">
+        <v>0</v>
+      </c>
+      <c r="E6" s="205" t="e">
         <f>'SFR ANALYSIS'!D39</f>
-        <v>133.09894525364138</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F6" s="220">
         <f>'SFR ANALYSIS'!I39</f>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G6" s="55"/>
       <c r="H6" s="61"/>
     </row>
     <row r="7" spans="1:13" ht="16" x14ac:dyDescent="0.15">
-      <c r="A7" s="391" t="str">
+      <c r="A7" s="395" t="str">
         <f>'SFR ANALYSIS'!A40</f>
         <v>N/A</v>
       </c>
-      <c r="B7" s="392"/>
+      <c r="B7" s="396"/>
       <c r="C7" s="206">
         <f>'SFR ANALYSIS'!B40</f>
         <v>0</v>
@@ -6461,7 +6496,7 @@
       </c>
       <c r="F7" s="221">
         <f>'SFR ANALYSIS'!I40</f>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="G7" s="61"/>
       <c r="H7" s="61"/>
@@ -6486,17 +6521,17 @@
       </c>
       <c r="F8" s="222">
         <f>'SFR ANALYSIS'!I41</f>
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="G8" s="61"/>
       <c r="H8" s="61"/>
     </row>
     <row r="9" spans="1:13" ht="16" x14ac:dyDescent="0.15">
-      <c r="A9" s="391" t="str">
+      <c r="A9" s="395" t="str">
         <f>'SFR ANALYSIS'!A42</f>
         <v>N/A</v>
       </c>
-      <c r="B9" s="392"/>
+      <c r="B9" s="396"/>
       <c r="C9" s="206">
         <f>'SFR ANALYSIS'!B42</f>
         <v>0</v>
@@ -6542,11 +6577,11 @@
       <c r="H10" s="61"/>
     </row>
     <row r="11" spans="1:13" ht="16" x14ac:dyDescent="0.15">
-      <c r="A11" s="391" t="str">
+      <c r="A11" s="395" t="str">
         <f>'SFR ANALYSIS'!A44</f>
         <v>N/A</v>
       </c>
-      <c r="B11" s="392"/>
+      <c r="B11" s="396"/>
       <c r="C11" s="206">
         <f>'SFR ANALYSIS'!B44</f>
         <v>0</v>
@@ -6592,11 +6627,11 @@
       <c r="H12" s="61"/>
     </row>
     <row r="13" spans="1:13" ht="16" x14ac:dyDescent="0.15">
-      <c r="A13" s="391" t="str">
+      <c r="A13" s="395" t="str">
         <f>'SFR ANALYSIS'!A46</f>
         <v>N/A</v>
       </c>
-      <c r="B13" s="392"/>
+      <c r="B13" s="396"/>
       <c r="C13" s="206">
         <f>'SFR ANALYSIS'!B46</f>
         <v>0</v>
@@ -6644,11 +6679,11 @@
       <c r="M14"/>
     </row>
     <row r="15" spans="1:13" ht="16" x14ac:dyDescent="0.15">
-      <c r="A15" s="391" t="str">
+      <c r="A15" s="395" t="str">
         <f>'SFR ANALYSIS'!A48</f>
         <v>N/A</v>
       </c>
-      <c r="B15" s="392"/>
+      <c r="B15" s="396"/>
       <c r="C15" s="206">
         <f>'SFR ANALYSIS'!B48</f>
         <v>0</v>
@@ -6700,8 +6735,8 @@
       <c r="M16"/>
     </row>
     <row r="17" spans="1:13" ht="14" x14ac:dyDescent="0.15">
-      <c r="A17" s="395"/>
-      <c r="B17" s="396"/>
+      <c r="A17" s="403"/>
+      <c r="B17" s="404"/>
       <c r="C17" s="208" t="s">
         <v>26</v>
       </c>
@@ -6719,21 +6754,21 @@
       <c r="M17"/>
     </row>
     <row r="18" spans="1:13" ht="16" x14ac:dyDescent="0.15">
-      <c r="A18" s="401" t="s">
-        <v>112</v>
-      </c>
-      <c r="B18" s="402"/>
-      <c r="C18" s="247">
+      <c r="A18" s="385" t="s">
+        <v>111</v>
+      </c>
+      <c r="B18" s="386"/>
+      <c r="C18" s="247" t="e">
         <f>'SFR ANALYSIS'!B51</f>
-        <v>265000</v>
-      </c>
-      <c r="D18" s="308">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D18" s="308" t="e">
         <f>'SFR ANALYSIS'!C51</f>
-        <v>1991</v>
-      </c>
-      <c r="E18" s="248">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E18" s="248" t="e">
         <f>'SFR ANALYSIS'!D51</f>
-        <v>133.09894525364138</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F18" s="225"/>
       <c r="G18" s="61"/>
@@ -6757,7 +6792,7 @@
     </row>
     <row r="20" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A20" s="233" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B20" s="210"/>
       <c r="C20" s="210"/>
@@ -6775,13 +6810,13 @@
         <v>11</v>
       </c>
       <c r="B21" s="211"/>
-      <c r="C21" s="315">
+      <c r="C21" s="315" t="e">
         <f>'SFR ANALYSIS'!B54</f>
-        <v>260341.53691612254</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="D21" s="316"/>
       <c r="E21" s="128" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F21" s="129">
         <f>'SFR ANALYSIS'!B23</f>
@@ -6792,7 +6827,7 @@
     </row>
     <row r="22" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="229" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B22" s="212"/>
       <c r="C22" s="367">
@@ -6804,7 +6839,7 @@
         <v>2</v>
       </c>
       <c r="E22" s="122" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F22" s="123">
         <f>'SFR ANALYSIS'!B24</f>
@@ -6815,7 +6850,7 @@
     </row>
     <row r="23" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A23" s="230" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B23" s="213"/>
       <c r="C23" s="214">
@@ -6824,11 +6859,11 @@
       </c>
       <c r="D23" s="215"/>
       <c r="E23" s="313" t="s">
-        <v>75</v>
-      </c>
-      <c r="F23" s="125">
+        <v>74</v>
+      </c>
+      <c r="F23" s="125" t="e">
         <f>'SFR ANALYSIS'!G51</f>
-        <v>30</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="G23" s="61"/>
       <c r="H23" s="61"/>
@@ -6845,7 +6880,7 @@
     </row>
     <row r="25" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A25" s="233" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B25" s="210"/>
       <c r="C25" s="210"/>
@@ -6857,7 +6892,7 @@
     </row>
     <row r="26" spans="1:13" ht="16" x14ac:dyDescent="0.15">
       <c r="A26" s="126" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B26" s="127"/>
       <c r="C26" s="128">
@@ -6866,7 +6901,7 @@
       </c>
       <c r="D26" s="128"/>
       <c r="E26" s="128" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F26" s="129">
         <f>'SFR ANALYSIS'!G54</f>
@@ -6877,7 +6912,7 @@
     </row>
     <row r="27" spans="1:13" ht="16" x14ac:dyDescent="0.15">
       <c r="A27" s="130" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B27" s="131"/>
       <c r="C27" s="121">
@@ -6886,7 +6921,7 @@
       </c>
       <c r="D27" s="121"/>
       <c r="E27" s="121" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F27" s="355">
         <f>'SFR ANALYSIS'!G55</f>
@@ -6897,7 +6932,7 @@
     </row>
     <row r="28" spans="1:13" ht="16" x14ac:dyDescent="0.15">
       <c r="A28" s="132" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B28" s="133"/>
       <c r="C28" s="96" t="str">
@@ -6906,7 +6941,7 @@
       </c>
       <c r="D28" s="96"/>
       <c r="E28" s="96" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F28" s="97">
         <f>'SFR ANALYSIS'!G56</f>
@@ -6917,7 +6952,7 @@
     </row>
     <row r="29" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A29" s="134" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B29" s="135"/>
       <c r="C29" s="173">
@@ -6926,7 +6961,7 @@
       </c>
       <c r="D29" s="136"/>
       <c r="E29" s="136" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F29" s="124">
         <f>'SFR ANALYSIS'!G57</f>
@@ -6947,17 +6982,17 @@
     </row>
     <row r="31" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A31" s="71" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B31" s="193"/>
       <c r="C31" s="244" t="s">
         <v>13</v>
       </c>
       <c r="D31" s="100" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E31" s="246" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F31" s="234"/>
       <c r="G31" s="61"/>
@@ -6965,7 +7000,7 @@
     </row>
     <row r="32" spans="1:13" ht="16" x14ac:dyDescent="0.15">
       <c r="A32" s="106" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B32" s="102"/>
       <c r="C32" s="174">
@@ -6986,13 +7021,13 @@
         <v>8</v>
       </c>
       <c r="B33" s="104"/>
-      <c r="C33" s="176">
+      <c r="C33" s="176" t="e">
         <f>'SFR ANALYSIS'!C76</f>
-        <v>15620.492214967351</v>
-      </c>
-      <c r="D33" s="179">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D33" s="179" t="e">
         <f>C33/C23</f>
-        <v>7.9859367152184824</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="E33" s="105">
         <f>'SFR ANALYSIS'!B76</f>
@@ -7007,13 +7042,13 @@
         <v>0</v>
       </c>
       <c r="B34" s="102"/>
-      <c r="C34" s="177">
+      <c r="C34" s="177" t="e">
         <f>'SFR ANALYSIS'!C77</f>
-        <v>7810.2461074836756</v>
-      </c>
-      <c r="D34" s="178">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D34" s="178" t="e">
         <f>C34/C23</f>
-        <v>3.9929683576092412</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="E34" s="107">
         <f>'SFR ANALYSIS'!B77</f>
@@ -7028,13 +7063,13 @@
         <v>9</v>
       </c>
       <c r="B35" s="104"/>
-      <c r="C35" s="176">
+      <c r="C35" s="176" t="e">
         <f>'SFR ANALYSIS'!C78</f>
-        <v>7810.2461074836756</v>
-      </c>
-      <c r="D35" s="179">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D35" s="179" t="e">
         <f>C35/C23</f>
-        <v>3.9929683576092412</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="E35" s="105">
         <f>'SFR ANALYSIS'!B78</f>
@@ -7064,16 +7099,16 @@
     </row>
     <row r="37" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A37" s="238" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B37" s="239"/>
-      <c r="C37" s="240">
+      <c r="C37" s="240" t="e">
         <f>'SFR ANALYSIS'!B84</f>
-        <v>134260.9844299347</v>
-      </c>
-      <c r="D37" s="241">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D37" s="241" t="e">
         <f>SUM(D32:D36)</f>
-        <v>68.640585086878687</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="E37" s="242"/>
       <c r="F37" s="243"/>
@@ -7099,13 +7134,13 @@
         <v>13</v>
       </c>
       <c r="D39" s="111" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E39" s="284" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F39" s="26" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G39" s="61"/>
       <c r="H39" s="61"/>
@@ -7115,9 +7150,9 @@
         <v>11</v>
       </c>
       <c r="B40" s="232"/>
-      <c r="C40" s="180">
+      <c r="C40" s="180" t="e">
         <f>'SFR ANALYSIS'!B100</f>
-        <v>260341.53691612254</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="D40" s="181">
         <f>C22</f>
@@ -7130,16 +7165,16 @@
     </row>
     <row r="41" spans="1:8" ht="16" x14ac:dyDescent="0.15">
       <c r="A41" s="113" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B41" s="199"/>
-      <c r="C41" s="182">
+      <c r="C41" s="182" t="e">
         <f>'SFR ANALYSIS'!B101</f>
-        <v>134260.9844299347</v>
-      </c>
-      <c r="D41" s="183">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D41" s="183" t="e">
         <f>D37</f>
-        <v>68.640585086878687</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="E41" s="195"/>
       <c r="F41" s="101"/>
@@ -7148,16 +7183,16 @@
     </row>
     <row r="42" spans="1:8" ht="16" x14ac:dyDescent="0.15">
       <c r="A42" s="137" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B42" s="200"/>
-      <c r="C42" s="180">
+      <c r="C42" s="180" t="e">
         <f>'SFR ANALYSIS'!B82</f>
-        <v>100046.39879457559</v>
-      </c>
-      <c r="D42" s="191">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D42" s="191" t="e">
         <f>C42/C23</f>
-        <v>51.148465641398566</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="E42" s="198"/>
       <c r="F42" s="237"/>
@@ -7166,16 +7201,16 @@
     </row>
     <row r="43" spans="1:8" ht="16" x14ac:dyDescent="0.15">
       <c r="A43" s="186" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B43" s="189"/>
-      <c r="C43" s="187">
+      <c r="C43" s="187" t="e">
         <f>SUM(C41:C42)</f>
-        <v>234307.3832245103</v>
-      </c>
-      <c r="D43" s="188">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D43" s="188" t="e">
         <f>C43/C23</f>
-        <v>119.78905072827725</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="E43" s="195"/>
       <c r="F43" s="101"/>
@@ -7193,19 +7228,19 @@
       <c r="H44" s="61"/>
     </row>
     <row r="45" spans="1:8" ht="16" x14ac:dyDescent="0.15">
-      <c r="A45" s="403" t="s">
-        <v>147</v>
-      </c>
-      <c r="B45" s="404"/>
-      <c r="C45" s="404"/>
-      <c r="D45" s="405"/>
+      <c r="A45" s="387" t="s">
+        <v>144</v>
+      </c>
+      <c r="B45" s="388"/>
+      <c r="C45" s="388"/>
+      <c r="D45" s="389"/>
       <c r="E45" s="365">
         <f>'SFR ANALYSIS'!B79</f>
         <v>0.1</v>
       </c>
-      <c r="F45" s="366">
+      <c r="F45" s="366" t="e">
         <f>'SFR ANALYSIS'!C79</f>
-        <v>26034.153691612257</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="G45" s="61"/>
       <c r="H45" s="61"/>
@@ -7250,14 +7285,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A8:B8"/>
     <mergeCell ref="A1:F2"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A16:B16"/>
@@ -7268,6 +7295,14 @@
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A8:B8"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>